<commit_message>
rede pública junto à rede privada
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -181,11 +181,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1524308172"/>
-        <c:axId val="751320217"/>
+        <c:axId val="1193856576"/>
+        <c:axId val="685843185"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1524308172"/>
+        <c:axId val="1193856576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -237,10 +237,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="751320217"/>
+        <c:crossAx val="685843185"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="751320217"/>
+        <c:axId val="685843185"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -315,7 +315,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1524308172"/>
+        <c:crossAx val="1193856576"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>